<commit_message>
add brands & change db
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" r:id="rId1"/>
@@ -971,15 +971,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -987,13 +987,16 @@
         <v>88</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1001,13 +1004,16 @@
         <v>5</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1018,10 +1024,13 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>23700</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1029,13 +1038,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>18950</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1046,10 +1058,13 @@
         <v>1</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>18950</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1057,13 +1072,16 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>23700</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1071,9 +1089,12 @@
         <v>4</v>
       </c>
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>680</v>
       </c>
     </row>
@@ -1363,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1689,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:J4"/>
+      <selection activeCell="C1" sqref="C1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,7 +1722,7 @@
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1709,31 +1730,28 @@
         <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1741,11 +1759,11 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>25650</v>
       </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
@@ -1756,16 +1774,13 @@
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>10170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1773,11 +1788,11 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
         <v>18950</v>
       </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
@@ -1788,16 +1803,13 @@
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3">
+      <c r="I3">
         <v>10171</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1805,11 +1817,11 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
         <v>44010</v>
       </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
@@ -1820,12 +1832,9 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="J4">
+      <c r="I4">
         <v>10172</v>
       </c>
     </row>

</xml_diff>